<commit_message>
before adding support for file changes
</commit_message>
<xml_diff>
--- a/M1K - FW Rule - Tracker.xlsx
+++ b/M1K - FW Rule - Tracker.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\firewall-request-qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7931FC99-DBF3-4B1B-823B-A32DCE018888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C503BD3-3AFF-416F-82BB-327EB3D7685D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34800" yWindow="-675" windowWidth="17280" windowHeight="9075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MasterProtected" sheetId="1" r:id="rId1"/>
-    <sheet name="FirewallRules" sheetId="2" r:id="rId2"/>
+    <sheet name="FirewallRulesToValidate" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>Source IP Description</t>
   </si>
@@ -98,6 +98,18 @@
   </si>
   <si>
     <t>30.0.0.0/16</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>10.108.0.1</t>
+  </si>
+  <si>
+    <t>20.0.0.1</t>
+  </si>
+  <si>
+    <t>22,  443</t>
   </si>
 </sst>
 </file>
@@ -448,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -780,15 +792,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F166D1D-84CF-41F3-9075-94983EF77A49}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" customWidth="1"/>
+    <col min="4" max="4" width="20.77734375" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -811,11 +833,172 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
support for comma seperated ips
</commit_message>
<xml_diff>
--- a/M1K - FW Rule - Tracker.xlsx
+++ b/M1K - FW Rule - Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\firewall-request-qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5A7CDC-F8B0-4246-912F-D74388276C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E48C12-6690-4765-943E-BC901D4E937F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="36">
   <si>
     <t>Source IP Description</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Azure Non prod</t>
   </si>
   <si>
-    <t>10.108.0.0/15</t>
-  </si>
-  <si>
     <t>IOD- Non-Prod</t>
   </si>
   <si>
@@ -100,9 +97,6 @@
     <t>30.0.0.0/16</t>
   </si>
   <si>
-    <t>10.108.0.1</t>
-  </si>
-  <si>
     <t>20.0.0.1</t>
   </si>
   <si>
@@ -122,6 +116,35 @@
   </si>
   <si>
     <t>10.201.0.1</t>
+  </si>
+  <si>
+    <t>10.108.0.0/15,
+10.110.64.0/22</t>
+  </si>
+  <si>
+    <t>10.110.64.0/22</t>
+  </si>
+  <si>
+    <t>30.0.0.1/32</t>
+  </si>
+  <si>
+    <t>HTTPS</t>
+  </si>
+  <si>
+    <t>20.0.0.1,30.0.0.1</t>
+  </si>
+  <si>
+    <t>200.0.32.0/22,
+10.110.64.1</t>
+  </si>
+  <si>
+    <t>udp</t>
+  </si>
+  <si>
+    <t>ICMP</t>
+  </si>
+  <si>
+    <t>icmp</t>
   </si>
 </sst>
 </file>
@@ -186,10 +209,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,7 +499,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -491,7 +517,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -521,36 +547,36 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -558,44 +584,32 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
@@ -836,7 +850,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -873,27 +887,27 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -901,64 +915,90 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="1">
         <v>3389</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1">
+        <v>443</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>

</xml_diff>

<commit_message>
adding support for port ranges
</commit_message>
<xml_diff>
--- a/M1K - FW Rule - Tracker.xlsx
+++ b/M1K - FW Rule - Tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\firewall-request-qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E48C12-6690-4765-943E-BC901D4E937F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A620802-C13D-4CAA-8C31-49480E28502D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="43">
   <si>
     <t>Source IP Description</t>
   </si>
@@ -107,9 +107,6 @@
   </si>
   <si>
     <t>SerialNo</t>
-  </si>
-  <si>
-    <t>Azure</t>
   </si>
   <si>
     <t>10.200.0.1</t>
@@ -145,6 +142,30 @@
   </si>
   <si>
     <t>icmp</t>
+  </si>
+  <si>
+    <t>Azure Non prod VM range</t>
+  </si>
+  <si>
+    <t>IOD- Non-Prod VM</t>
+  </si>
+  <si>
+    <t>22-25,  443</t>
+  </si>
+  <si>
+    <t>22-100,  3389</t>
+  </si>
+  <si>
+    <t>10.108.0.1</t>
+  </si>
+  <si>
+    <t>http</t>
+  </si>
+  <si>
+    <t>80-105</t>
+  </si>
+  <si>
+    <t>101-105</t>
   </si>
 </sst>
 </file>
@@ -499,7 +520,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,7 +530,7 @@
     <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.33203125" customWidth="1"/>
     <col min="10" max="10" width="11.21875" bestFit="1" customWidth="1"/>
@@ -555,7 +576,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>10</v>
@@ -564,10 +585,10 @@
         <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>13</v>
@@ -850,17 +871,17 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="1" max="1" width="25.44140625" customWidth="1"/>
     <col min="2" max="2" width="21.88671875" customWidth="1"/>
-    <col min="3" max="3" width="15.77734375" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" customWidth="1"/>
     <col min="4" max="4" width="20.77734375" customWidth="1"/>
     <col min="5" max="5" width="11.109375" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
     <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -889,22 +910,22 @@
     </row>
     <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>13</v>
@@ -912,13 +933,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>20</v>
@@ -935,16 +956,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>11</v>
@@ -958,16 +979,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>11</v>
@@ -976,65 +997,121 @@
         <v>443</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="1">
+        <v>80</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="1">
+        <v>101</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>

</xml_diff>